<commit_message>
20171208 修正Google Excel問題單 第77條
</commit_message>
<xml_diff>
--- a/templates/組長作業區-每日筆數統計.xlsx
+++ b/templates/組長作業區-每日筆數統計.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>行家</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -34,51 +34,35 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>報機單(袋數)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>${table:data.W2_BAG_COUNT}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>報機單(小號數)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>${table:data.W2_COUNT}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${table:data.W3_COUNT}</t>
+    <t>報機單(份數)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>${table:data.OL_W2_COUNT}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${table:data.W1_COUNT}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>報機單(袋數)</t>
+    <t>銷倉單(份數)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>銷倉單(袋數)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>派送單(袋數)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>報機單(件數)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>銷倉單(件數)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>派送單(件數)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>${table:data.W1_BAG_COUNT}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>${table:data.W3_BAG_COUNT}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>${table:data.W2_BAG_COUNT}</t>
+    <t>${table:data.OL_W3_COUNT}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -459,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -472,54 +456,40 @@
     <col min="3" max="3" width="26.5" customWidth="1"/>
     <col min="4" max="4" width="26.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
-    <col min="6" max="6" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1">
+    <row r="1" spans="1:5" s="3" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>